<commit_message>
Div ROE e ROIC
</commit_message>
<xml_diff>
--- a/Ações_Mágicas.xlsx
+++ b/Ações_Mágicas.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://8zdvht.sharepoint.com/sites/INVESTIMENTOS/Documentos Compartilhados/Scripts de Análise de ações/App_web_Análise_Fundamentalista_Ações/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_DBF588DA9CDFD54CA84C4D3F61CAA63710838183" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0DB5C136-AD41-4776-96D6-B169D713DD4B}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -559,8 +565,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -623,13 +629,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -667,7 +681,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -701,6 +715,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -735,9 +750,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -910,14 +926,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J103"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -949,7 +967,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -963,13 +981,13 @@
         <v>4.32</v>
       </c>
       <c r="E2">
-        <v>19.99</v>
+        <v>19.989999999999998</v>
       </c>
       <c r="F2">
         <v>38.97</v>
       </c>
       <c r="G2">
-        <v>4.929057</v>
+        <v>4.9290570000000002</v>
       </c>
       <c r="H2">
         <v>16.43019</v>
@@ -981,7 +999,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -1013,7 +1031,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -1033,10 +1051,10 @@
         <v>28.58</v>
       </c>
       <c r="G4">
-        <v>1.869466</v>
+        <v>1.8694660000000001</v>
       </c>
       <c r="H4">
-        <v>6.231553333333334</v>
+        <v>6.2315533333333342</v>
       </c>
       <c r="I4" t="s">
         <v>114</v>
@@ -1045,7 +1063,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -1065,10 +1083,10 @@
         <v>0</v>
       </c>
       <c r="G5">
-        <v>17.509593</v>
+        <v>17.509592999999999</v>
       </c>
       <c r="H5">
-        <v>58.36531000000002</v>
+        <v>58.365310000000022</v>
       </c>
       <c r="I5" t="s">
         <v>115</v>
@@ -1077,12 +1095,12 @@
         <v>125</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>14</v>
       </c>
       <c r="B6">
-        <v>35.34</v>
+        <v>35.340000000000003</v>
       </c>
       <c r="C6">
         <v>28.71</v>
@@ -1097,10 +1115,10 @@
         <v>16.13</v>
       </c>
       <c r="G6">
-        <v>17.67382</v>
+        <v>17.673819999999999</v>
       </c>
       <c r="H6">
-        <v>58.91273333333334</v>
+        <v>58.912733333333343</v>
       </c>
       <c r="I6" t="s">
         <v>114</v>
@@ -1109,12 +1127,12 @@
         <v>126</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>15</v>
       </c>
       <c r="B7">
-        <v>2.26</v>
+        <v>2.2599999999999998</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -1141,7 +1159,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -1158,13 +1176,13 @@
         <v>28.07</v>
       </c>
       <c r="F8">
-        <v>16.06</v>
+        <v>16.059999999999999</v>
       </c>
       <c r="G8">
-        <v>0.490248</v>
+        <v>0.49024800000000002</v>
       </c>
       <c r="H8">
-        <v>1.63416</v>
+        <v>1.6341600000000001</v>
       </c>
       <c r="I8" t="s">
         <v>114</v>
@@ -1173,7 +1191,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -1193,7 +1211,7 @@
         <v>17.47</v>
       </c>
       <c r="G9">
-        <v>3.553792</v>
+        <v>3.5537920000000001</v>
       </c>
       <c r="H9">
         <v>11.84597333333333</v>
@@ -1205,7 +1223,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -1228,7 +1246,7 @@
         <v>5.209714</v>
       </c>
       <c r="H10">
-        <v>17.36571333333333</v>
+        <v>17.365713333333328</v>
       </c>
       <c r="I10" t="s">
         <v>117</v>
@@ -1237,7 +1255,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -1260,7 +1278,7 @@
         <v>12.391159</v>
       </c>
       <c r="H11">
-        <v>41.30386333333333</v>
+        <v>41.303863333333332</v>
       </c>
       <c r="I11" t="s">
         <v>115</v>
@@ -1269,7 +1287,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -1280,7 +1298,7 @@
         <v>10.33</v>
       </c>
       <c r="D12">
-        <v>8.789999999999999</v>
+        <v>8.7899999999999991</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -1292,7 +1310,7 @@
         <v>11.129991</v>
       </c>
       <c r="H12">
-        <v>37.09997000000001</v>
+        <v>37.099970000000013</v>
       </c>
       <c r="I12" t="s">
         <v>115</v>
@@ -1301,7 +1319,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -1315,16 +1333,16 @@
         <v>8.27</v>
       </c>
       <c r="E13">
-        <v>10.03</v>
+        <v>10.029999999999999</v>
       </c>
       <c r="F13">
         <v>13.98</v>
       </c>
       <c r="G13">
-        <v>10.584737</v>
+        <v>10.584737000000001</v>
       </c>
       <c r="H13">
-        <v>35.28245666666667</v>
+        <v>35.282456666666668</v>
       </c>
       <c r="I13" t="s">
         <v>117</v>
@@ -1333,7 +1351,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -1356,7 +1374,7 @@
         <v>0.752</v>
       </c>
       <c r="H14">
-        <v>2.506666666666667</v>
+        <v>2.5066666666666668</v>
       </c>
       <c r="I14" t="s">
         <v>116</v>
@@ -1365,7 +1383,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -1385,10 +1403,10 @@
         <v>23.32</v>
       </c>
       <c r="G15">
-        <v>30.127007</v>
+        <v>30.127006999999999</v>
       </c>
       <c r="H15">
-        <v>100.4233566666666</v>
+        <v>100.42335666666661</v>
       </c>
       <c r="I15" t="s">
         <v>112</v>
@@ -1397,7 +1415,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -1417,10 +1435,10 @@
         <v>10.61</v>
       </c>
       <c r="G16">
-        <v>0.890081</v>
+        <v>0.89008100000000001</v>
       </c>
       <c r="H16">
-        <v>2.966936666666667</v>
+        <v>2.9669366666666672</v>
       </c>
       <c r="I16" t="s">
         <v>112</v>
@@ -1429,7 +1447,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>25</v>
       </c>
@@ -1440,16 +1458,16 @@
         <v>0.16</v>
       </c>
       <c r="D17">
-        <v>8.960000000000001</v>
+        <v>8.9600000000000009</v>
       </c>
       <c r="E17">
-        <v>73.98999999999999</v>
+        <v>73.989999999999995</v>
       </c>
       <c r="F17">
         <v>44.93</v>
       </c>
       <c r="G17">
-        <v>0.072644</v>
+        <v>7.2644E-2</v>
       </c>
       <c r="H17">
         <v>0.2421466666666667</v>
@@ -1461,7 +1479,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>26</v>
       </c>
@@ -1481,10 +1499,10 @@
         <v>12.71</v>
       </c>
       <c r="G18">
-        <v>7.479182</v>
+        <v>7.4791819999999998</v>
       </c>
       <c r="H18">
-        <v>24.93060666666667</v>
+        <v>24.930606666666669</v>
       </c>
       <c r="I18" t="s">
         <v>118</v>
@@ -1493,7 +1511,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>27</v>
       </c>
@@ -1501,10 +1519,10 @@
         <v>7.05</v>
       </c>
       <c r="C19">
-        <v>4.14</v>
+        <v>4.1399999999999997</v>
       </c>
       <c r="D19">
-        <v>8.140000000000001</v>
+        <v>8.14</v>
       </c>
       <c r="E19">
         <v>22.48</v>
@@ -1516,7 +1534,7 @@
         <v>0.72175</v>
       </c>
       <c r="H19">
-        <v>2.405833333333334</v>
+        <v>2.4058333333333342</v>
       </c>
       <c r="I19" t="s">
         <v>114</v>
@@ -1525,7 +1543,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>28</v>
       </c>
@@ -1533,7 +1551,7 @@
         <v>20.14</v>
       </c>
       <c r="C20">
-        <v>4.64</v>
+        <v>4.6399999999999997</v>
       </c>
       <c r="D20">
         <v>8.77</v>
@@ -1548,7 +1566,7 @@
         <v>1.654493</v>
       </c>
       <c r="H20">
-        <v>5.514976666666667</v>
+        <v>5.5149766666666666</v>
       </c>
       <c r="I20" t="s">
         <v>114</v>
@@ -1557,7 +1575,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>29</v>
       </c>
@@ -1565,7 +1583,7 @@
         <v>21.72</v>
       </c>
       <c r="C21">
-        <v>4.56</v>
+        <v>4.5599999999999996</v>
       </c>
       <c r="D21">
         <v>6.84</v>
@@ -1577,10 +1595,10 @@
         <v>32.08</v>
       </c>
       <c r="G21">
-        <v>1.764844</v>
+        <v>1.7648440000000001</v>
       </c>
       <c r="H21">
-        <v>5.882813333333334</v>
+        <v>5.8828133333333339</v>
       </c>
       <c r="I21" t="s">
         <v>113</v>
@@ -1589,7 +1607,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>30</v>
       </c>
@@ -1609,10 +1627,10 @@
         <v>23.48</v>
       </c>
       <c r="G22">
-        <v>0.9132399999999999</v>
+        <v>0.91323999999999994</v>
       </c>
       <c r="H22">
-        <v>3.044133333333333</v>
+        <v>3.0441333333333329</v>
       </c>
       <c r="I22" t="s">
         <v>118</v>
@@ -1621,7 +1639,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>31</v>
       </c>
@@ -1641,7 +1659,7 @@
         <v>18.8</v>
       </c>
       <c r="G23">
-        <v>1.025078</v>
+        <v>1.0250779999999999</v>
       </c>
       <c r="H23">
         <v>3.416926666666666</v>
@@ -1653,7 +1671,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>32</v>
       </c>
@@ -1670,7 +1688,7 @@
         <v>24.11</v>
       </c>
       <c r="F24">
-        <v>16.83</v>
+        <v>16.829999999999998</v>
       </c>
       <c r="G24">
         <v>0</v>
@@ -1685,7 +1703,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>33</v>
       </c>
@@ -1708,7 +1726,7 @@
         <v>12.792171</v>
       </c>
       <c r="H25">
-        <v>42.64057</v>
+        <v>42.640569999999997</v>
       </c>
       <c r="I25" t="s">
         <v>117</v>
@@ -1717,7 +1735,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>34</v>
       </c>
@@ -1737,7 +1755,7 @@
         <v>14.58</v>
       </c>
       <c r="G26">
-        <v>3.657109</v>
+        <v>3.6571090000000002</v>
       </c>
       <c r="H26">
         <v>12.19036333333333</v>
@@ -1749,7 +1767,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>35</v>
       </c>
@@ -1769,10 +1787,10 @@
         <v>11.32</v>
       </c>
       <c r="G27">
-        <v>9.079999000000001</v>
+        <v>9.0799990000000008</v>
       </c>
       <c r="H27">
-        <v>30.26666333333334</v>
+        <v>30.266663333333341</v>
       </c>
       <c r="I27" t="s">
         <v>112</v>
@@ -1781,7 +1799,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>36</v>
       </c>
@@ -1801,10 +1819,10 @@
         <v>13.68</v>
       </c>
       <c r="G28">
-        <v>28.782801</v>
+        <v>28.782800999999999</v>
       </c>
       <c r="H28">
-        <v>95.94267000000001</v>
+        <v>95.942670000000007</v>
       </c>
       <c r="I28" t="s">
         <v>112</v>
@@ -1813,7 +1831,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>37</v>
       </c>
@@ -1833,7 +1851,7 @@
         <v>11.8</v>
       </c>
       <c r="G29">
-        <v>3.019985</v>
+        <v>3.0199850000000001</v>
       </c>
       <c r="H29">
         <v>10.06661666666667</v>
@@ -1845,7 +1863,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>38</v>
       </c>
@@ -1868,7 +1886,7 @@
         <v>2.233841</v>
       </c>
       <c r="H30">
-        <v>7.446136666666667</v>
+        <v>7.4461366666666668</v>
       </c>
       <c r="I30" t="s">
         <v>118</v>
@@ -1877,7 +1895,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>39</v>
       </c>
@@ -1900,7 +1918,7 @@
         <v>6.44</v>
       </c>
       <c r="H31">
-        <v>21.46666666666667</v>
+        <v>21.466666666666669</v>
       </c>
       <c r="I31" t="s">
         <v>112</v>
@@ -1909,12 +1927,12 @@
         <v>143</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>40</v>
       </c>
       <c r="B32">
-        <v>4.69</v>
+        <v>4.6900000000000004</v>
       </c>
       <c r="C32">
         <v>4.63</v>
@@ -1923,7 +1941,7 @@
         <v>6.09</v>
       </c>
       <c r="E32">
-        <v>-4.31</v>
+        <v>-4.3099999999999996</v>
       </c>
       <c r="F32">
         <v>31.88</v>
@@ -1932,7 +1950,7 @@
         <v>2.573995</v>
       </c>
       <c r="H32">
-        <v>8.579983333333335</v>
+        <v>8.5799833333333346</v>
       </c>
       <c r="I32" t="s">
         <v>119</v>
@@ -1941,7 +1959,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>41</v>
       </c>
@@ -1949,7 +1967,7 @@
         <v>12.45</v>
       </c>
       <c r="C33">
-        <v>2.55</v>
+        <v>2.5499999999999998</v>
       </c>
       <c r="D33">
         <v>9.57</v>
@@ -1961,10 +1979,10 @@
         <v>5.27</v>
       </c>
       <c r="G33">
-        <v>1.153631</v>
+        <v>1.1536310000000001</v>
       </c>
       <c r="H33">
-        <v>3.845436666666667</v>
+        <v>3.8454366666666671</v>
       </c>
       <c r="I33" t="s">
         <v>116</v>
@@ -1973,7 +1991,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>42</v>
       </c>
@@ -1996,7 +2014,7 @@
         <v>1.903551</v>
       </c>
       <c r="H34">
-        <v>6.34517</v>
+        <v>6.3451700000000004</v>
       </c>
       <c r="I34" t="s">
         <v>115</v>
@@ -2005,7 +2023,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>43</v>
       </c>
@@ -2025,10 +2043,10 @@
         <v>12.2</v>
       </c>
       <c r="G35">
-        <v>6.762532</v>
+        <v>6.7625320000000002</v>
       </c>
       <c r="H35">
-        <v>22.54177333333334</v>
+        <v>22.541773333333339</v>
       </c>
       <c r="I35" t="s">
         <v>116</v>
@@ -2037,7 +2055,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>44</v>
       </c>
@@ -2060,7 +2078,7 @@
         <v>1.212737</v>
       </c>
       <c r="H36">
-        <v>4.042456666666666</v>
+        <v>4.0424566666666664</v>
       </c>
       <c r="I36" t="s">
         <v>117</v>
@@ -2069,7 +2087,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>45</v>
       </c>
@@ -2083,16 +2101,16 @@
         <v>8.51</v>
       </c>
       <c r="E37">
-        <v>17.19</v>
+        <v>17.190000000000001</v>
       </c>
       <c r="F37">
         <v>19.59</v>
       </c>
       <c r="G37">
-        <v>5.877085</v>
+        <v>5.8770850000000001</v>
       </c>
       <c r="H37">
-        <v>19.59028333333333</v>
+        <v>19.590283333333328</v>
       </c>
       <c r="I37" t="s">
         <v>112</v>
@@ -2101,7 +2119,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="38" spans="1:10">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>46</v>
       </c>
@@ -2115,16 +2133,16 @@
         <v>6.03</v>
       </c>
       <c r="E38">
-        <v>8.529999999999999</v>
+        <v>8.5299999999999994</v>
       </c>
       <c r="F38">
         <v>18.47</v>
       </c>
       <c r="G38">
-        <v>6.139445</v>
+        <v>6.1394450000000003</v>
       </c>
       <c r="H38">
-        <v>20.46481666666667</v>
+        <v>20.464816666666671</v>
       </c>
       <c r="I38" t="s">
         <v>117</v>
@@ -2133,7 +2151,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="39" spans="1:10">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>47</v>
       </c>
@@ -2144,7 +2162,7 @@
         <v>5.95</v>
       </c>
       <c r="D39">
-        <v>9.470000000000001</v>
+        <v>9.4700000000000006</v>
       </c>
       <c r="E39">
         <v>6.28</v>
@@ -2156,7 +2174,7 @@
         <v>3.031946</v>
       </c>
       <c r="H39">
-        <v>10.10648666666667</v>
+        <v>10.106486666666671</v>
       </c>
       <c r="I39" t="s">
         <v>119</v>
@@ -2165,7 +2183,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="40" spans="1:10">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>48</v>
       </c>
@@ -2185,10 +2203,10 @@
         <v>193.3</v>
       </c>
       <c r="G40">
-        <v>3.020422</v>
+        <v>3.0204219999999999</v>
       </c>
       <c r="H40">
-        <v>10.06807333333333</v>
+        <v>10.068073333333331</v>
       </c>
       <c r="I40" t="s">
         <v>116</v>
@@ -2197,7 +2215,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="41" spans="1:10">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>49</v>
       </c>
@@ -2208,7 +2226,7 @@
         <v>4.91</v>
       </c>
       <c r="D41">
-        <v>8.550000000000001</v>
+        <v>8.5500000000000007</v>
       </c>
       <c r="E41">
         <v>15.92</v>
@@ -2217,7 +2235,7 @@
         <v>7.12</v>
       </c>
       <c r="G41">
-        <v>7.520694</v>
+        <v>7.5206939999999998</v>
       </c>
       <c r="H41">
         <v>25.06898</v>
@@ -2229,7 +2247,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="42" spans="1:10">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>50</v>
       </c>
@@ -2249,10 +2267,10 @@
         <v>23.35</v>
       </c>
       <c r="G42">
-        <v>1.776377</v>
+        <v>1.7763770000000001</v>
       </c>
       <c r="H42">
-        <v>5.921256666666667</v>
+        <v>5.9212566666666673</v>
       </c>
       <c r="I42" t="s">
         <v>120</v>
@@ -2261,7 +2279,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="43" spans="1:10">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>51</v>
       </c>
@@ -2278,13 +2296,13 @@
         <v>14.26</v>
       </c>
       <c r="F43">
-        <v>10.13</v>
+        <v>10.130000000000001</v>
       </c>
       <c r="G43">
         <v>2.759887</v>
       </c>
       <c r="H43">
-        <v>9.199623333333333</v>
+        <v>9.1996233333333333</v>
       </c>
       <c r="I43" t="s">
         <v>117</v>
@@ -2293,7 +2311,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="44" spans="1:10">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>52</v>
       </c>
@@ -2304,7 +2322,7 @@
         <v>5.92</v>
       </c>
       <c r="D44">
-        <v>9.880000000000001</v>
+        <v>9.8800000000000008</v>
       </c>
       <c r="E44">
         <v>48.68</v>
@@ -2325,7 +2343,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="45" spans="1:10">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>53</v>
       </c>
@@ -2348,7 +2366,7 @@
         <v>0.130468</v>
       </c>
       <c r="H45">
-        <v>0.4348933333333334</v>
+        <v>0.43489333333333341</v>
       </c>
       <c r="I45" t="s">
         <v>112</v>
@@ -2357,7 +2375,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="46" spans="1:10">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>54</v>
       </c>
@@ -2377,10 +2395,10 @@
         <v>0</v>
       </c>
       <c r="G46">
-        <v>0.162184</v>
+        <v>0.16218399999999999</v>
       </c>
       <c r="H46">
-        <v>0.5406133333333334</v>
+        <v>0.54061333333333339</v>
       </c>
       <c r="I46" t="s">
         <v>115</v>
@@ -2389,7 +2407,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="47" spans="1:10">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>55</v>
       </c>
@@ -2397,7 +2415,7 @@
         <v>28.84</v>
       </c>
       <c r="C47">
-        <v>4.36</v>
+        <v>4.3600000000000003</v>
       </c>
       <c r="D47">
         <v>9.09</v>
@@ -2409,10 +2427,10 @@
         <v>0</v>
       </c>
       <c r="G47">
-        <v>6.974987999999999</v>
+        <v>6.9749879999999989</v>
       </c>
       <c r="H47">
-        <v>23.24996</v>
+        <v>23.249960000000002</v>
       </c>
       <c r="I47" t="s">
         <v>115</v>
@@ -2421,7 +2439,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="48" spans="1:10">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>56</v>
       </c>
@@ -2441,10 +2459,10 @@
         <v>5.48</v>
       </c>
       <c r="G48">
-        <v>1.536912</v>
+        <v>1.5369120000000001</v>
       </c>
       <c r="H48">
-        <v>5.12304</v>
+        <v>5.1230399999999996</v>
       </c>
       <c r="I48" t="s">
         <v>119</v>
@@ -2453,7 +2471,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="49" spans="1:10">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>57</v>
       </c>
@@ -2467,16 +2485,16 @@
         <v>13.94</v>
       </c>
       <c r="E49">
-        <v>-9.630000000000001</v>
+        <v>-9.6300000000000008</v>
       </c>
       <c r="F49">
-        <v>17.76</v>
+        <v>17.760000000000002</v>
       </c>
       <c r="G49">
-        <v>2.08709</v>
+        <v>2.0870899999999999</v>
       </c>
       <c r="H49">
-        <v>6.956966666666666</v>
+        <v>6.9569666666666663</v>
       </c>
       <c r="I49" t="s">
         <v>112</v>
@@ -2485,7 +2503,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="50" spans="1:10">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>58</v>
       </c>
@@ -2502,13 +2520,13 @@
         <v>11.69</v>
       </c>
       <c r="F50">
-        <v>17.81</v>
+        <v>17.809999999999999</v>
       </c>
       <c r="G50">
-        <v>3.265163</v>
+        <v>3.2651629999999998</v>
       </c>
       <c r="H50">
-        <v>10.88387666666667</v>
+        <v>10.883876666666669</v>
       </c>
       <c r="I50" t="s">
         <v>115</v>
@@ -2517,7 +2535,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="51" spans="1:10">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>59</v>
       </c>
@@ -2549,7 +2567,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="52" spans="1:10">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>60</v>
       </c>
@@ -2560,7 +2578,7 @@
         <v>0</v>
       </c>
       <c r="D52">
-        <v>4.85</v>
+        <v>4.8499999999999996</v>
       </c>
       <c r="E52">
         <v>14.44</v>
@@ -2569,10 +2587,10 @@
         <v>5.2</v>
       </c>
       <c r="G52">
-        <v>0.017136</v>
+        <v>1.7135999999999998E-2</v>
       </c>
       <c r="H52">
-        <v>0.05712</v>
+        <v>5.7119999999999997E-2</v>
       </c>
       <c r="I52" t="s">
         <v>114</v>
@@ -2581,7 +2599,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="53" spans="1:10">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>61</v>
       </c>
@@ -2589,7 +2607,7 @@
         <v>25.04</v>
       </c>
       <c r="C53">
-        <v>4.6</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="D53">
         <v>7.26</v>
@@ -2601,7 +2619,7 @@
         <v>0</v>
       </c>
       <c r="G53">
-        <v>5.63181</v>
+        <v>5.6318099999999998</v>
       </c>
       <c r="H53">
         <v>18.7727</v>
@@ -2613,7 +2631,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="54" spans="1:10">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>62</v>
       </c>
@@ -2627,16 +2645,16 @@
         <v>11.7</v>
       </c>
       <c r="E54">
-        <v>20.26</v>
+        <v>20.260000000000002</v>
       </c>
       <c r="F54">
         <v>7.18</v>
       </c>
       <c r="G54">
-        <v>0.8046810000000001</v>
+        <v>0.80468100000000009</v>
       </c>
       <c r="H54">
-        <v>2.68227</v>
+        <v>2.6822699999999999</v>
       </c>
       <c r="I54" t="s">
         <v>116</v>
@@ -2645,7 +2663,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="55" spans="1:10">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>63</v>
       </c>
@@ -2659,7 +2677,7 @@
         <v>11.69</v>
       </c>
       <c r="E55">
-        <v>-17.92</v>
+        <v>-17.920000000000002</v>
       </c>
       <c r="F55">
         <v>145.07</v>
@@ -2668,7 +2686,7 @@
         <v>1.559385</v>
       </c>
       <c r="H55">
-        <v>5.197950000000001</v>
+        <v>5.1979500000000014</v>
       </c>
       <c r="I55" t="s">
         <v>118</v>
@@ -2677,7 +2695,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="56" spans="1:10">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>64</v>
       </c>
@@ -2697,10 +2715,10 @@
         <v>17.59</v>
       </c>
       <c r="G56">
-        <v>0.456012</v>
+        <v>0.45601199999999997</v>
       </c>
       <c r="H56">
-        <v>1.52004</v>
+        <v>1.5200400000000001</v>
       </c>
       <c r="I56" t="s">
         <v>114</v>
@@ -2709,7 +2727,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="57" spans="1:10">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>65</v>
       </c>
@@ -2720,19 +2738,19 @@
         <v>5.95</v>
       </c>
       <c r="D57">
-        <v>8.289999999999999</v>
+        <v>8.2899999999999991</v>
       </c>
       <c r="E57">
         <v>1.44</v>
       </c>
       <c r="F57">
-        <v>9.720000000000001</v>
+        <v>9.7200000000000006</v>
       </c>
       <c r="G57">
-        <v>3.158047</v>
+        <v>3.1580469999999998</v>
       </c>
       <c r="H57">
-        <v>10.52682333333333</v>
+        <v>10.526823333333329</v>
       </c>
       <c r="I57" t="s">
         <v>116</v>
@@ -2741,7 +2759,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="58" spans="1:10">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>66</v>
       </c>
@@ -2752,10 +2770,10 @@
         <v>2.57</v>
       </c>
       <c r="D58">
-        <v>9.300000000000001</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="E58">
-        <v>9.369999999999999</v>
+        <v>9.3699999999999992</v>
       </c>
       <c r="F58">
         <v>23.17</v>
@@ -2764,7 +2782,7 @@
         <v>1.520197</v>
       </c>
       <c r="H58">
-        <v>5.067323333333333</v>
+        <v>5.0673233333333334</v>
       </c>
       <c r="I58" t="s">
         <v>120</v>
@@ -2773,12 +2791,12 @@
         <v>159</v>
       </c>
     </row>
-    <row r="59" spans="1:10">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>67</v>
       </c>
       <c r="B59">
-        <v>36.91</v>
+        <v>36.909999999999997</v>
       </c>
       <c r="C59">
         <v>1.67</v>
@@ -2790,13 +2808,13 @@
         <v>27.1</v>
       </c>
       <c r="F59">
-        <v>16.6</v>
+        <v>16.600000000000001</v>
       </c>
       <c r="G59">
-        <v>1.881592</v>
+        <v>1.8815919999999999</v>
       </c>
       <c r="H59">
-        <v>6.271973333333333</v>
+        <v>6.2719733333333334</v>
       </c>
       <c r="I59" t="s">
         <v>116</v>
@@ -2805,7 +2823,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="60" spans="1:10">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>68</v>
       </c>
@@ -2828,7 +2846,7 @@
         <v>1.261099</v>
       </c>
       <c r="H60">
-        <v>4.203663333333333</v>
+        <v>4.2036633333333331</v>
       </c>
       <c r="I60" t="s">
         <v>119</v>
@@ -2837,7 +2855,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="61" spans="1:10">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>69</v>
       </c>
@@ -2854,10 +2872,10 @@
         <v>24.39</v>
       </c>
       <c r="F61">
-        <v>18.4</v>
+        <v>18.399999999999999</v>
       </c>
       <c r="G61">
-        <v>9.869229000000001</v>
+        <v>9.8692290000000007</v>
       </c>
       <c r="H61">
         <v>32.89743</v>
@@ -2869,7 +2887,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="62" spans="1:10">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>70</v>
       </c>
@@ -2892,7 +2910,7 @@
         <v>11.507555</v>
       </c>
       <c r="H62">
-        <v>38.35851666666667</v>
+        <v>38.358516666666667</v>
       </c>
       <c r="I62" t="s">
         <v>117</v>
@@ -2901,12 +2919,12 @@
         <v>162</v>
       </c>
     </row>
-    <row r="63" spans="1:10">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>71</v>
       </c>
       <c r="B63">
-        <v>38.38</v>
+        <v>38.380000000000003</v>
       </c>
       <c r="C63">
         <v>7.59</v>
@@ -2921,7 +2939,7 @@
         <v>44.57</v>
       </c>
       <c r="G63">
-        <v>15.594499</v>
+        <v>15.594499000000001</v>
       </c>
       <c r="H63">
         <v>51.98166333333333</v>
@@ -2933,7 +2951,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="64" spans="1:10">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>72</v>
       </c>
@@ -2965,7 +2983,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="65" spans="1:10">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>73</v>
       </c>
@@ -2985,10 +3003,10 @@
         <v>12.67</v>
       </c>
       <c r="G65">
-        <v>9.892620000000001</v>
+        <v>9.8926200000000009</v>
       </c>
       <c r="H65">
-        <v>32.97540000000001</v>
+        <v>32.975400000000008</v>
       </c>
       <c r="I65" t="s">
         <v>112</v>
@@ -2997,7 +3015,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="66" spans="1:10">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>74</v>
       </c>
@@ -3017,7 +3035,7 @@
         <v>40.19</v>
       </c>
       <c r="G66">
-        <v>2.136535</v>
+        <v>2.1365349999999999</v>
       </c>
       <c r="H66">
         <v>7.121783333333334</v>
@@ -3029,7 +3047,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="67" spans="1:10">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>75</v>
       </c>
@@ -3037,7 +3055,7 @@
         <v>13.58</v>
       </c>
       <c r="C67">
-        <v>2.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="D67">
         <v>13.67</v>
@@ -3049,10 +3067,10 @@
         <v>18.3</v>
       </c>
       <c r="G67">
-        <v>0.7477240000000001</v>
+        <v>0.74772400000000006</v>
       </c>
       <c r="H67">
-        <v>2.492413333333333</v>
+        <v>2.4924133333333329</v>
       </c>
       <c r="I67" t="s">
         <v>116</v>
@@ -3061,7 +3079,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="68" spans="1:10">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>76</v>
       </c>
@@ -3069,22 +3087,22 @@
         <v>37.61</v>
       </c>
       <c r="C68">
-        <v>2.07</v>
+        <v>2.0699999999999998</v>
       </c>
       <c r="D68">
         <v>16.32</v>
       </c>
       <c r="E68">
-        <v>35.34</v>
+        <v>35.340000000000003</v>
       </c>
       <c r="F68">
         <v>0</v>
       </c>
       <c r="G68">
-        <v>2.521607</v>
+        <v>2.5216069999999999</v>
       </c>
       <c r="H68">
-        <v>8.405356666666668</v>
+        <v>8.4053566666666679</v>
       </c>
       <c r="I68" t="s">
         <v>115</v>
@@ -3093,7 +3111,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="69" spans="1:10">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>77</v>
       </c>
@@ -3113,10 +3131,10 @@
         <v>5.99</v>
       </c>
       <c r="G69">
-        <v>2.555451</v>
+        <v>2.5554510000000001</v>
       </c>
       <c r="H69">
-        <v>8.518170000000001</v>
+        <v>8.5181700000000014</v>
       </c>
       <c r="I69" t="s">
         <v>116</v>
@@ -3125,7 +3143,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="70" spans="1:10">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>78</v>
       </c>
@@ -3142,13 +3160,13 @@
         <v>29.26</v>
       </c>
       <c r="F70">
-        <v>18.65</v>
+        <v>18.649999999999999</v>
       </c>
       <c r="G70">
-        <v>0.91543</v>
+        <v>0.91542999999999997</v>
       </c>
       <c r="H70">
-        <v>3.051433333333333</v>
+        <v>3.0514333333333332</v>
       </c>
       <c r="I70" t="s">
         <v>114</v>
@@ -3157,7 +3175,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="71" spans="1:10">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>79</v>
       </c>
@@ -3177,10 +3195,10 @@
         <v>1.74</v>
       </c>
       <c r="G71">
-        <v>1.925317</v>
+        <v>1.9253169999999999</v>
       </c>
       <c r="H71">
-        <v>6.417723333333335</v>
+        <v>6.4177233333333348</v>
       </c>
       <c r="I71" t="s">
         <v>113</v>
@@ -3189,12 +3207,12 @@
         <v>169</v>
       </c>
     </row>
-    <row r="72" spans="1:10">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>80</v>
       </c>
       <c r="B72">
-        <v>18.85</v>
+        <v>18.850000000000001</v>
       </c>
       <c r="C72">
         <v>1.37</v>
@@ -3209,10 +3227,10 @@
         <v>5.83</v>
       </c>
       <c r="G72">
-        <v>0.446316</v>
+        <v>0.44631599999999999</v>
       </c>
       <c r="H72">
-        <v>1.48772</v>
+        <v>1.4877199999999999</v>
       </c>
       <c r="I72" t="s">
         <v>116</v>
@@ -3221,7 +3239,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="73" spans="1:10">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>81</v>
       </c>
@@ -3241,10 +3259,10 @@
         <v>1.58</v>
       </c>
       <c r="G73">
-        <v>0.396396</v>
+        <v>0.39639600000000003</v>
       </c>
       <c r="H73">
-        <v>1.32132</v>
+        <v>1.3213200000000001</v>
       </c>
       <c r="I73" t="s">
         <v>117</v>
@@ -3253,7 +3271,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="74" spans="1:10">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>82</v>
       </c>
@@ -3273,7 +3291,7 @@
         <v>14.17</v>
       </c>
       <c r="G74">
-        <v>1.106556</v>
+        <v>1.1065560000000001</v>
       </c>
       <c r="H74">
         <v>3.68852</v>
@@ -3285,12 +3303,12 @@
         <v>152</v>
       </c>
     </row>
-    <row r="75" spans="1:10">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>83</v>
       </c>
       <c r="B75">
-        <v>9.369999999999999</v>
+        <v>9.3699999999999992</v>
       </c>
       <c r="C75">
         <v>4.71</v>
@@ -3308,7 +3326,7 @@
         <v>1.367807</v>
       </c>
       <c r="H75">
-        <v>4.559356666666668</v>
+        <v>4.5593566666666678</v>
       </c>
       <c r="I75" t="s">
         <v>116</v>
@@ -3317,7 +3335,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="76" spans="1:10">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>84</v>
       </c>
@@ -3337,7 +3355,7 @@
         <v>21.64</v>
       </c>
       <c r="G76">
-        <v>6.655499</v>
+        <v>6.6554989999999998</v>
       </c>
       <c r="H76">
         <v>22.18499666666667</v>
@@ -3349,7 +3367,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="77" spans="1:10">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>85</v>
       </c>
@@ -3369,10 +3387,10 @@
         <v>1.28</v>
       </c>
       <c r="G77">
-        <v>0.322458</v>
+        <v>0.32245800000000002</v>
       </c>
       <c r="H77">
-        <v>1.07486</v>
+        <v>1.0748599999999999</v>
       </c>
       <c r="I77" t="s">
         <v>118</v>
@@ -3381,7 +3399,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="78" spans="1:10">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>86</v>
       </c>
@@ -3404,7 +3422,7 @@
         <v>1.634752</v>
       </c>
       <c r="H78">
-        <v>5.449173333333333</v>
+        <v>5.4491733333333334</v>
       </c>
       <c r="I78" t="s">
         <v>114</v>
@@ -3413,7 +3431,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="79" spans="1:10">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>87</v>
       </c>
@@ -3433,10 +3451,10 @@
         <v>3.7</v>
       </c>
       <c r="G79">
-        <v>4.229102999999999</v>
+        <v>4.2291029999999994</v>
       </c>
       <c r="H79">
-        <v>14.09701</v>
+        <v>14.097009999999999</v>
       </c>
       <c r="I79" t="s">
         <v>116</v>
@@ -3445,7 +3463,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="80" spans="1:10">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>88</v>
       </c>
@@ -3477,7 +3495,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="81" spans="1:10">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>89</v>
       </c>
@@ -3497,7 +3515,7 @@
         <v>21.23</v>
       </c>
       <c r="G81">
-        <v>2.969243</v>
+        <v>2.9692430000000001</v>
       </c>
       <c r="H81">
         <v>9.897476666666666</v>
@@ -3509,7 +3527,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="82" spans="1:10">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>90</v>
       </c>
@@ -3520,7 +3538,7 @@
         <v>3.62</v>
       </c>
       <c r="D82">
-        <v>19.35</v>
+        <v>19.350000000000001</v>
       </c>
       <c r="E82">
         <v>-14.64</v>
@@ -3529,10 +3547,10 @@
         <v>17.07</v>
       </c>
       <c r="G82">
-        <v>3.919407</v>
+        <v>3.9194070000000001</v>
       </c>
       <c r="H82">
-        <v>13.06469</v>
+        <v>13.064690000000001</v>
       </c>
       <c r="I82" t="s">
         <v>116</v>
@@ -3541,7 +3559,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="83" spans="1:10">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>91</v>
       </c>
@@ -3561,10 +3579,10 @@
         <v>15.19</v>
       </c>
       <c r="G83">
-        <v>5.437291999999999</v>
+        <v>5.4372919999999993</v>
       </c>
       <c r="H83">
-        <v>18.12430666666667</v>
+        <v>18.124306666666669</v>
       </c>
       <c r="I83" t="s">
         <v>114</v>
@@ -3573,7 +3591,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="84" spans="1:10">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>92</v>
       </c>
@@ -3593,10 +3611,10 @@
         <v>1.24</v>
       </c>
       <c r="G84">
-        <v>7.286282999999999</v>
+        <v>7.2862829999999992</v>
       </c>
       <c r="H84">
-        <v>24.28761</v>
+        <v>24.287610000000001</v>
       </c>
       <c r="I84" t="s">
         <v>114</v>
@@ -3605,7 +3623,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="85" spans="1:10">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>93</v>
       </c>
@@ -3625,10 +3643,10 @@
         <v>3.34</v>
       </c>
       <c r="G85">
-        <v>1.008663</v>
+        <v>1.0086630000000001</v>
       </c>
       <c r="H85">
-        <v>3.36221</v>
+        <v>3.3622100000000001</v>
       </c>
       <c r="I85" t="s">
         <v>120</v>
@@ -3637,7 +3655,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="86" spans="1:10">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>94</v>
       </c>
@@ -3660,7 +3678,7 @@
         <v>12.779881</v>
       </c>
       <c r="H86">
-        <v>42.59960333333333</v>
+        <v>42.599603333333327</v>
       </c>
       <c r="I86" t="s">
         <v>118</v>
@@ -3669,7 +3687,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="87" spans="1:10">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>95</v>
       </c>
@@ -3689,10 +3707,10 @@
         <v>15.27</v>
       </c>
       <c r="G87">
-        <v>0.322398</v>
+        <v>0.32239800000000002</v>
       </c>
       <c r="H87">
-        <v>1.07466</v>
+        <v>1.0746599999999999</v>
       </c>
       <c r="I87" t="s">
         <v>121</v>
@@ -3701,7 +3719,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="88" spans="1:10">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>96</v>
       </c>
@@ -3721,10 +3739,10 @@
         <v>8.25</v>
       </c>
       <c r="G88">
-        <v>8.467643000000001</v>
+        <v>8.4676430000000007</v>
       </c>
       <c r="H88">
-        <v>28.22547666666667</v>
+        <v>28.225476666666669</v>
       </c>
       <c r="I88" t="s">
         <v>117</v>
@@ -3733,12 +3751,12 @@
         <v>141</v>
       </c>
     </row>
-    <row r="89" spans="1:10">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>97</v>
       </c>
       <c r="B89">
-        <v>8.449999999999999</v>
+        <v>8.4499999999999993</v>
       </c>
       <c r="C89">
         <v>3.44</v>
@@ -3753,10 +3771,10 @@
         <v>2.56</v>
       </c>
       <c r="G89">
-        <v>1.24137</v>
+        <v>1.2413700000000001</v>
       </c>
       <c r="H89">
-        <v>4.1379</v>
+        <v>4.1379000000000001</v>
       </c>
       <c r="I89" t="s">
         <v>118</v>
@@ -3765,7 +3783,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="90" spans="1:10">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>98</v>
       </c>
@@ -3785,7 +3803,7 @@
         <v>18.72</v>
       </c>
       <c r="G90">
-        <v>1.303195</v>
+        <v>1.3031950000000001</v>
       </c>
       <c r="H90">
         <v>4.343983333333334</v>
@@ -3797,7 +3815,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="91" spans="1:10">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>99</v>
       </c>
@@ -3817,10 +3835,10 @@
         <v>0</v>
       </c>
       <c r="G91">
-        <v>4.621130000000001</v>
+        <v>4.6211300000000008</v>
       </c>
       <c r="H91">
-        <v>15.40376666666667</v>
+        <v>15.403766666666669</v>
       </c>
       <c r="I91" t="s">
         <v>115</v>
@@ -3829,7 +3847,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="92" spans="1:10">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>100</v>
       </c>
@@ -3861,7 +3879,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="93" spans="1:10">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>101</v>
       </c>
@@ -3881,10 +3899,10 @@
         <v>37.94</v>
       </c>
       <c r="G93">
-        <v>4.915384</v>
+        <v>4.9153840000000004</v>
       </c>
       <c r="H93">
-        <v>16.38461333333333</v>
+        <v>16.384613333333331</v>
       </c>
       <c r="I93" t="s">
         <v>117</v>
@@ -3893,7 +3911,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="94" spans="1:10">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>102</v>
       </c>
@@ -3913,10 +3931,10 @@
         <v>10.72</v>
       </c>
       <c r="G94">
-        <v>0.8105559999999999</v>
+        <v>0.81055599999999994</v>
       </c>
       <c r="H94">
-        <v>2.701853333333333</v>
+        <v>2.7018533333333332</v>
       </c>
       <c r="I94" t="s">
         <v>116</v>
@@ -3925,7 +3943,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="95" spans="1:10">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>103</v>
       </c>
@@ -3948,7 +3966,7 @@
         <v>5.047663</v>
       </c>
       <c r="H95">
-        <v>16.82554333333334</v>
+        <v>16.825543333333339</v>
       </c>
       <c r="I95" t="s">
         <v>115</v>
@@ -3957,7 +3975,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="96" spans="1:10">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>104</v>
       </c>
@@ -3974,13 +3992,13 @@
         <v>37.49</v>
       </c>
       <c r="F96">
-        <v>8.109999999999999</v>
+        <v>8.11</v>
       </c>
       <c r="G96">
-        <v>7.39075</v>
+        <v>7.3907499999999997</v>
       </c>
       <c r="H96">
-        <v>24.63583333333333</v>
+        <v>24.635833333333331</v>
       </c>
       <c r="I96" t="s">
         <v>114</v>
@@ -3989,7 +4007,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="97" spans="1:10">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>105</v>
       </c>
@@ -4009,10 +4027,10 @@
         <v>12.29</v>
       </c>
       <c r="G97">
-        <v>4.8054</v>
+        <v>4.8053999999999997</v>
       </c>
       <c r="H97">
-        <v>16.018</v>
+        <v>16.018000000000001</v>
       </c>
       <c r="I97" t="s">
         <v>117</v>
@@ -4021,7 +4039,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="98" spans="1:10">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>106</v>
       </c>
@@ -4032,7 +4050,7 @@
         <v>1</v>
       </c>
       <c r="D98">
-        <v>35.02</v>
+        <v>35.020000000000003</v>
       </c>
       <c r="E98">
         <v>184.64</v>
@@ -4041,7 +4059,7 @@
         <v>13.57</v>
       </c>
       <c r="G98">
-        <v>0.6448269999999999</v>
+        <v>0.64482699999999993</v>
       </c>
       <c r="H98">
         <v>2.149423333333333</v>
@@ -4053,12 +4071,12 @@
         <v>166</v>
       </c>
     </row>
-    <row r="99" spans="1:10">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>107</v>
       </c>
       <c r="B99">
-        <v>17.42</v>
+        <v>17.420000000000002</v>
       </c>
       <c r="C99">
         <v>4.13</v>
@@ -4073,10 +4091,10 @@
         <v>6.95</v>
       </c>
       <c r="G99">
-        <v>2.681496</v>
+        <v>2.6814960000000001</v>
       </c>
       <c r="H99">
-        <v>8.938319999999999</v>
+        <v>8.9383199999999992</v>
       </c>
       <c r="I99" t="s">
         <v>114</v>
@@ -4085,7 +4103,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="100" spans="1:10">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>108</v>
       </c>
@@ -4093,7 +4111,7 @@
         <v>29.02</v>
       </c>
       <c r="C100">
-        <v>0.29</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="D100">
         <v>20.27</v>
@@ -4117,7 +4135,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:10">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>109</v>
       </c>
@@ -4149,7 +4167,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="102" spans="1:10">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>110</v>
       </c>
@@ -4169,10 +4187,10 @@
         <v>7.06</v>
       </c>
       <c r="G102">
-        <v>2.140089</v>
+        <v>2.1400890000000001</v>
       </c>
       <c r="H102">
-        <v>7.13363</v>
+        <v>7.1336300000000001</v>
       </c>
       <c r="I102" t="s">
         <v>117</v>
@@ -4181,7 +4199,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="103" spans="1:10">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>111</v>
       </c>
@@ -4201,10 +4219,10 @@
         <v>21.52</v>
       </c>
       <c r="G103">
-        <v>0.453738</v>
+        <v>0.45373799999999997</v>
       </c>
       <c r="H103">
-        <v>1.51246</v>
+        <v>1.5124599999999999</v>
       </c>
       <c r="I103" t="s">
         <v>114</v>
@@ -4219,6 +4237,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100C1E5D1EB1B65964C845AF9732F46C499" ma:contentTypeVersion="9" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="53da220994c263061237558b4b19d7e9">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="94331225-a384-4379-98f7-51cdceba5e43" xmlns:ns3="2da23abd-c153-46ca-9656-d51f60595101" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9771c53ab827f697218d6811cc07834c" ns2:_="" ns3:_="">
     <xsd:import namespace="94331225-a384-4379-98f7-51cdceba5e43"/>
@@ -4401,19 +4428,29 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8C2A0E10-80F8-4CA1-80C3-963077F1F242}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5264BD26-2076-49F4-8E69-AE86883A420C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5264BD26-2076-49F4-8E69-AE86883A420C}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8C2A0E10-80F8-4CA1-80C3-963077F1F242}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="94331225-a384-4379-98f7-51cdceba5e43"/>
+    <ds:schemaRef ds:uri="2da23abd-c153-46ca-9656-d51f60595101"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>